<commit_message>
updated status, brightness input card done
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_25_Mar.xlsx
+++ b/other/Project_TimeLine_2021_25_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0BF8E48-3121-4FBF-843A-DAF600BB228F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ECEFF1-FDE5-4F58-A24D-26327DCE0DA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
   <si>
     <t>S/N</t>
   </si>
@@ -148,10 +148,15 @@
     <t>Pop-up itself is done but lacks functionality to access and use it</t>
   </si>
   <si>
-    <t>Currently working on it, might delay other tasks slightly</t>
-  </si>
-  <si>
     <t>Front-end: Edit light location button in table</t>
+  </si>
+  <si>
+    <t>On hold as I think it's better to finish cleaning up the code first 
+before adding this feature</t>
+  </si>
+  <si>
+    <t>Completed dashboard and config page. With the exception of
+user management, remaining pages should be trivial.</t>
   </si>
 </sst>
 </file>
@@ -535,7 +540,7 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -978,12 +983,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -997,18 +1002,27 @@
       <c r="F19" s="3">
         <v>44278</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="H19" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" t="s">
-        <v>37</v>
-      </c>
-      <c r="I21" s="4" t="s">
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3">
+        <v>44273</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="4" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
left with cleaning custom calendar
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_25_Mar.xlsx
+++ b/other/Project_TimeLine_2021_25_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38ECEFF1-FDE5-4F58-A24D-26327DCE0DA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61121AEB-2711-4D43-869F-D87990C8A5CD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -539,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,8 +1016,14 @@
       <c r="C20" t="s">
         <v>8</v>
       </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
       <c r="E20" s="3">
         <v>44273</v>
+      </c>
+      <c r="F20" s="3">
+        <v>44284</v>
       </c>
       <c r="H20" s="4" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
updated reports, fixed table element padding, added relocation button to card
</commit_message>
<xml_diff>
--- a/other/Project_TimeLine_2021_25_Mar.xlsx
+++ b/other/Project_TimeLine_2021_25_Mar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Murphy Tan\Desktop\aztech-lms\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15F42579-82FB-4EEA-A36F-7D87D6C1BBCC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5487EDE-5BE2-47A8-8BBB-5BAD1E713C35}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{5A8E5395-CCD6-4F57-83A8-81B53FE4AFF6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>S/N</t>
   </si>
@@ -139,10 +139,6 @@
   </si>
   <si>
     <t>Code refactoring</t>
-  </si>
-  <si>
-    <t>Code is becoming really
-messy (especially CSS). Would have to clean up for better scalability.</t>
   </si>
   <si>
     <t>Pop-up itself is done but lacks functionality to access and use it</t>
@@ -153,10 +149,6 @@
   <si>
     <t>On hold as I think it's better to finish cleaning up the code first 
 before adding this feature</t>
-  </si>
-  <si>
-    <t>Completed dashboard and config page. With the exception of
-user management, remaining pages should be trivial.</t>
   </si>
 </sst>
 </file>
@@ -539,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4C0DE7D-B314-4018-AC47-8A93F1174983}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,7 +972,7 @@
         <v>44272</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="45" x14ac:dyDescent="0.25">
@@ -988,7 +980,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -1003,10 +995,10 @@
         <v>44278</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1025,12 +1017,11 @@
       <c r="F20" s="3">
         <v>44284</v>
       </c>
-      <c r="H20" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="I20" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="G20" s="3">
+        <v>44284</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
     </row>
     <row r="26" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B26" t="s">

</xml_diff>